<commit_message>
remove error from vocabulary and update json version
</commit_message>
<xml_diff>
--- a/storage/app/keywords/1-2/240214 MSL vocabulary Material.xlsx
+++ b/storage/app/keywords/1-2/240214 MSL vocabulary Material.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/r_p_j_pijnenburg_uu_nl/Documents/EPOS-NL/07 Data/Metadata/231212 MSL vocabs 1.2 - update but not yet implemented/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsh001\Projects\epos\storage\app\keywords\1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="519" documentId="8_{F56B2338-6F22-4B08-988B-943DD4C3EDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1451D30-A770-473C-87D9-8C6685F68375}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5161C069-615D-416C-95C7-EAC928FD16CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="734" xr2:uid="{5382AC07-EECC-46C6-ADAA-955BBC56FF66}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="734" xr2:uid="{5382AC07-EECC-46C6-ADAA-955BBC56FF66}"/>
   </bookViews>
   <sheets>
     <sheet name="2021 sample material" sheetId="10" r:id="rId1"/>
@@ -2110,7 +2110,7 @@
     <t>clay - kaolinite #kaolinite</t>
   </si>
   <si>
-    <t>silicone #silly putty #sillyputty# polydimethylsiloxane PDMS #SiliconSilly puttyPDMS #PDMS #Silicon Silly putty   PDMSImages of histological sections of oocytes to quantify oocyte size frequency distributions in Astarte crenata and Ctenodiscus crispatus used in the analyses by Reed et al. 2021 (Ecology and Evolution) from the Western Barents Sea during summer 2017 across a North - South transect intersecting the polar front. Supported by The Changing Arctic Ocean Seafloor (ChAOS) - how changing sea ice conditions impact biological communities, biogeochemical processes and ecosystems project (NE/N015894/1 and NE/P006426/1, 2017-2021), Natural Environment Research Council (NERC) in the UK.</t>
+    <t>silicone #silly putty #sillyputty# polydimethylsiloxane PDMS #SiliconSilly puttyPDMS #PDMS #Silicon Silly putty</t>
   </si>
 </sst>
 </file>
@@ -2659,10 +2659,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2964,22 +2960,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A651" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D659" sqref="D654:E659"/>
+      <selection pane="bottomLeft" activeCell="E661" sqref="E661"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="4" width="35.44140625" customWidth="1"/>
-    <col min="5" max="5" width="49.109375" customWidth="1"/>
-    <col min="6" max="6" width="29.44140625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" customWidth="1"/>
-    <col min="9" max="9" width="44.33203125" customWidth="1"/>
+    <col min="3" max="4" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="9" max="9" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="18.75">
       <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
@@ -4966,14 +4962,14 @@
         <v>217</v>
       </c>
     </row>
-    <row r="288" spans="2:7" ht="15.6">
+    <row r="288" spans="2:7" ht="15.75">
       <c r="C288" s="10" t="s">
         <v>218</v>
       </c>
       <c r="E288" s="1"/>
       <c r="F288" s="1"/>
     </row>
-    <row r="289" spans="3:6" ht="15.6">
+    <row r="289" spans="3:6" ht="15.75">
       <c r="C289" s="10" t="s">
         <v>219</v>
       </c>
@@ -4990,21 +4986,21 @@
         <v>221</v>
       </c>
     </row>
-    <row r="292" spans="3:6" ht="15.6">
+    <row r="292" spans="3:6" ht="15.75">
       <c r="C292" s="10" t="s">
         <v>222</v>
       </c>
       <c r="E292" s="1"/>
       <c r="F292" s="1"/>
     </row>
-    <row r="293" spans="3:6" ht="15.6">
+    <row r="293" spans="3:6" ht="15.75">
       <c r="C293" s="10" t="s">
         <v>223</v>
       </c>
       <c r="E293" s="1"/>
       <c r="F293" s="1"/>
     </row>
-    <row r="294" spans="3:6" ht="15.6">
+    <row r="294" spans="3:6" ht="15.75">
       <c r="C294" s="10" t="s">
         <v>224</v>
       </c>
@@ -5126,28 +5122,28 @@
         <v>247</v>
       </c>
     </row>
-    <row r="318" spans="3:6" ht="15.6">
+    <row r="318" spans="3:6" ht="15.75">
       <c r="C318" s="10" t="s">
         <v>248</v>
       </c>
       <c r="E318" s="1"/>
       <c r="F318" s="1"/>
     </row>
-    <row r="319" spans="3:6" ht="15.6">
+    <row r="319" spans="3:6" ht="15.75">
       <c r="C319" s="10" t="s">
         <v>249</v>
       </c>
       <c r="E319" s="1"/>
       <c r="F319" s="1"/>
     </row>
-    <row r="320" spans="3:6" ht="15.6">
+    <row r="320" spans="3:6" ht="15.75">
       <c r="C320" s="10" t="s">
         <v>250</v>
       </c>
       <c r="E320" s="1"/>
       <c r="F320" s="1"/>
     </row>
-    <row r="321" spans="2:6" ht="15.6">
+    <row r="321" spans="2:6" ht="15.75">
       <c r="C321" s="10" t="s">
         <v>251</v>
       </c>
@@ -6753,7 +6749,7 @@
       <c r="E607" s="47"/>
       <c r="F607" s="17"/>
     </row>
-    <row r="608" spans="1:6" ht="28.8">
+    <row r="608" spans="1:6" ht="30">
       <c r="A608" s="48"/>
       <c r="B608" s="47"/>
       <c r="D608" s="47" t="s">
@@ -7086,7 +7082,7 @@
       </c>
       <c r="E645" s="47"/>
     </row>
-    <row r="646" spans="1:5">
+    <row r="646" spans="1:5" ht="30">
       <c r="A646" s="48"/>
       <c r="B646" s="47"/>
       <c r="C646" s="47"/>
@@ -7104,7 +7100,7 @@
       </c>
       <c r="E647" s="47"/>
     </row>
-    <row r="648" spans="1:5">
+    <row r="648" spans="1:5" ht="30">
       <c r="A648" s="48"/>
       <c r="B648" s="47"/>
       <c r="C648" s="47"/>
@@ -7113,7 +7109,7 @@
       </c>
       <c r="E648" s="47"/>
     </row>
-    <row r="649" spans="1:5" ht="28.8">
+    <row r="649" spans="1:5" ht="30">
       <c r="A649" s="48"/>
       <c r="B649" s="47"/>
       <c r="C649" s="47"/>
@@ -7167,7 +7163,7 @@
       </c>
       <c r="E654" s="47"/>
     </row>
-    <row r="655" spans="1:5" ht="28.8">
+    <row r="655" spans="1:5" ht="30">
       <c r="A655" s="48"/>
       <c r="B655" s="47"/>
       <c r="C655" s="47"/>
@@ -7176,7 +7172,7 @@
       </c>
       <c r="E655" s="47"/>
     </row>
-    <row r="656" spans="1:5" ht="28.8">
+    <row r="656" spans="1:5" ht="30">
       <c r="A656" s="48"/>
       <c r="B656" s="47" t="s">
         <v>589</v>
@@ -7215,7 +7211,7 @@
       </c>
       <c r="E660" s="47"/>
     </row>
-    <row r="661" spans="1:5" ht="273.60000000000002">
+    <row r="661" spans="1:5" ht="60">
       <c r="B661" s="47"/>
       <c r="C661" s="47"/>
       <c r="D661" s="47" t="s">
@@ -7990,12 +7986,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="53df6a5f-9334-4503-a845-5e05459a4c71" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2184524c-f8db-481f-81f4-afb1a4d0a68c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8247,29 +8245,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="53df6a5f-9334-4503-a845-5e05459a4c71" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2184524c-f8db-481f-81f4-afb1a4d0a68c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2045B72B-3B0C-4673-8101-B1CED3BDCC66}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6960850B-255D-4E63-83A0-9FA77F00B90D}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA8759FF-6AD2-4D1A-A25A-9AED9AEB8089}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8278,4 +8262,32 @@
     <ds:schemaRef ds:uri="2184524c-f8db-481f-81f4-afb1a4d0a68c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6960850B-255D-4E63-83A0-9FA77F00B90D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2184524c-f8db-481f-81f4-afb1a4d0a68c"/>
+    <ds:schemaRef ds:uri="53df6a5f-9334-4503-a845-5e05459a4c71"/>
+    <ds:schemaRef ds:uri="6965ef5a-98c2-4976-9e1e-bc6458d0e33d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2045B72B-3B0C-4673-8101-B1CED3BDCC66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>